<commit_message>
changed excel file to have separate sheets per member
</commit_message>
<xml_diff>
--- a/report/dummy.xlsx
+++ b/report/dummy.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishek/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C1AEB22-B715-494D-A7E8-0448E3258EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A59F7F-EA7F-C94D-B07C-4CA957EDE0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{67EA143E-9FE8-7540-9204-94FEFE791C20}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{67EA143E-9FE8-7540-9204-94FEFE791C20}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Team" sheetId="1" r:id="rId1"/>
+    <sheet name="George" sheetId="2" r:id="rId2"/>
+    <sheet name="Abhishek" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,6 +35,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -404,7 +410,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A65ED4-AFC3-7943-A54F-D26BF1B03A96}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2032B162-400A-904A-9AB6-0D1C6A289E88}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AF9D12-BAE8-1A42-83B7-3859D323A59F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>